<commit_message>
Algunos cálculos de lambda
Da pena.
</commit_message>
<xml_diff>
--- a/TP1/resultados raíces.xlsx
+++ b/TP1/resultados raíces.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lukas\Desktop\Numérico\TP1\Analisis_Numerico_fiuba\TP1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC423856-B784-41D9-A4AE-3F1D29FBF6D9}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DADBFB3-F6BD-44DB-A91D-8DC97A340A0D}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="24">
   <si>
     <t>im</t>
   </si>
@@ -90,13 +90,16 @@
     <t>Resultado</t>
   </si>
   <si>
-    <t xml:space="preserve"> </t>
+    <t>Lambda</t>
   </si>
   <si>
-    <t>Alfa</t>
+    <t>Alfa =</t>
   </si>
   <si>
-    <t>Lambda</t>
+    <t>Miren esos números, dan lástima.</t>
+  </si>
+  <si>
+    <t>Ya estoy harto de este tp.</t>
   </si>
 </sst>
 </file>
@@ -105,7 +108,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.00000000"/>
-    <numFmt numFmtId="171" formatCode="0.0000000000"/>
+    <numFmt numFmtId="165" formatCode="0.0000000000"/>
   </numFmts>
   <fonts count="19" x14ac:knownFonts="1">
     <font>
@@ -251,7 +254,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="33">
+  <fills count="34">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -429,6 +432,12 @@
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.39997558519241921"/>
         <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -592,11 +601,19 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Énfasis1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -952,42 +969,48 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J175"/>
+  <dimension ref="A1:L175"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="L8" sqref="L8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="18.5703125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="12.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="15.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
+      <c r="B1" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2">
+        <f>B29</f>
+        <v>1.4142135600000001</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="E1" s="1">
+        <f>D28</f>
+        <v>1.709511279572963</v>
+      </c>
+      <c r="G1" t="s">
         <v>20</v>
       </c>
-      <c r="D1" t="s">
-        <v>21</v>
-      </c>
-      <c r="F1" t="s">
-        <v>22</v>
-      </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>18</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>0</v>
       </c>
@@ -995,14 +1018,14 @@
         <v>1</v>
       </c>
       <c r="D2" s="1"/>
-      <c r="I2">
+      <c r="J2">
         <v>0</v>
       </c>
-      <c r="J2" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K2" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
       </c>
@@ -1010,14 +1033,14 @@
         <v>1.5</v>
       </c>
       <c r="D3" s="1"/>
-      <c r="I3">
-        <v>1</v>
-      </c>
-      <c r="J3" s="1">
+      <c r="J3">
+        <v>1</v>
+      </c>
+      <c r="K3" s="1">
         <v>1.39413027</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2</v>
       </c>
@@ -1029,14 +1052,18 @@
         <v>1</v>
       </c>
       <c r="F4" s="3"/>
-      <c r="I4">
+      <c r="G4">
+        <f xml:space="preserve"> ABS(B5-C$1) / (ABS(B4-C$1) ^ D4)</f>
+        <v>0.23879611403589368</v>
+      </c>
+      <c r="J4">
         <v>2</v>
       </c>
-      <c r="J4" s="1">
+      <c r="K4" s="1">
         <v>1.876493</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>3</v>
       </c>
@@ -1048,14 +1075,18 @@
         <v>1</v>
       </c>
       <c r="E5" s="3"/>
-      <c r="I5">
+      <c r="G5">
+        <f t="shared" ref="G5:G28" si="1" xml:space="preserve"> ABS(B6-C$1) / (ABS(B5-C$1) ^ D5)</f>
+        <v>0.59383641781056995</v>
+      </c>
+      <c r="J5">
         <v>3</v>
       </c>
-      <c r="J5" s="1">
+      <c r="K5" s="1">
         <v>1.5492468399999999</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>4</v>
       </c>
@@ -1066,14 +1097,18 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="I6">
+      <c r="G6">
+        <f t="shared" si="1"/>
+        <v>0.34198271612149056</v>
+      </c>
+      <c r="J6">
         <v>4</v>
       </c>
-      <c r="J6" s="1">
+      <c r="K6" s="1">
         <v>1.4523931400000001</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>5</v>
       </c>
@@ -1084,14 +1119,18 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="I7">
+      <c r="G7">
+        <f t="shared" si="1"/>
+        <v>0.96206219329041531</v>
+      </c>
+      <c r="J7">
         <v>5</v>
       </c>
-      <c r="J7" s="1">
+      <c r="K7" s="1">
         <v>1.50001538</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>6</v>
       </c>
@@ -1102,14 +1141,19 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="I8">
+      <c r="G8">
+        <f t="shared" si="1"/>
+        <v>1.9716920056816144E-2</v>
+      </c>
+      <c r="J8">
         <v>6</v>
       </c>
-      <c r="J8" s="1">
+      <c r="K8" s="1">
         <v>1.49999986</v>
       </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L8" s="3"/>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>7</v>
       </c>
@@ -1120,14 +1164,18 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="I9">
+      <c r="G9">
+        <f t="shared" si="1"/>
+        <v>24.858930226384413</v>
+      </c>
+      <c r="J9">
         <v>7</v>
       </c>
-      <c r="J9" s="1">
+      <c r="K9" s="1">
         <v>1.5</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>8</v>
       </c>
@@ -1139,8 +1187,12 @@
         <v>0.99999630670544515</v>
       </c>
       <c r="F10" s="1"/>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="G10">
+        <f t="shared" si="1"/>
+        <v>0.4798752744214016</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>9</v>
       </c>
@@ -1152,8 +1204,12 @@
         <v>1.0000110799340407</v>
       </c>
       <c r="F11" s="1"/>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="G11">
+        <f t="shared" si="1"/>
+        <v>0.45811892892751988</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>10</v>
       </c>
@@ -1165,8 +1221,12 @@
         <v>0.99999261345566892</v>
       </c>
       <c r="F12" s="1"/>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="G12" s="3">
+        <f t="shared" si="1"/>
+        <v>0.40848251524350532</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>11</v>
       </c>
@@ -1178,8 +1238,12 @@
         <v>1.0000000000009841</v>
       </c>
       <c r="F13" s="1"/>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="G13">
+        <f t="shared" si="1"/>
+        <v>0.27602158828255369</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>12</v>
       </c>
@@ -1191,8 +1255,17 @@
         <v>0.99999999999934386</v>
       </c>
       <c r="F14" s="1"/>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="G14">
+        <f t="shared" si="1"/>
+        <v>0.31145251396632584</v>
+      </c>
+      <c r="I14" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="J14" s="7"/>
+      <c r="K14" s="7"/>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>13</v>
       </c>
@@ -1204,8 +1277,17 @@
         <v>0.99988181895843031</v>
       </c>
       <c r="F15" s="1"/>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="G15">
+        <f t="shared" si="1"/>
+        <v>1.1041893201204753</v>
+      </c>
+      <c r="I15" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="J15" s="7"/>
+      <c r="K15" s="7"/>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>14</v>
       </c>
@@ -1217,8 +1299,12 @@
         <v>1.0001181950047304</v>
       </c>
       <c r="F16" s="1"/>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G16">
+        <f t="shared" si="1"/>
+        <v>4.7796333810119503E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>15</v>
       </c>
@@ -1230,8 +1316,12 @@
         <v>1.0000000000262406</v>
       </c>
       <c r="F17" s="1"/>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G17">
+        <f t="shared" si="1"/>
+        <v>8.9738562134748996</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>16</v>
       </c>
@@ -1243,8 +1333,12 @@
         <v>0.99999999995801525</v>
       </c>
       <c r="F18" s="1"/>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G18">
+        <f t="shared" si="1"/>
+        <v>0.44428259265269437</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>17</v>
       </c>
@@ -1256,8 +1350,12 @@
         <v>1.0018920593927649</v>
       </c>
       <c r="F19" s="1"/>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G19">
+        <f t="shared" si="1"/>
+        <v>0.38403615513827433</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>18</v>
       </c>
@@ -1269,8 +1367,12 @@
         <v>0.99433701481292647</v>
       </c>
       <c r="F20" s="1"/>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G20">
+        <f t="shared" si="1"/>
+        <v>0.15417286617477352</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>19</v>
       </c>
@@ -1282,8 +1384,12 @@
         <v>1.0113979631778283</v>
       </c>
       <c r="F21" s="1"/>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G21">
+        <f t="shared" si="1"/>
+        <v>1.7752873111145009</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>20</v>
       </c>
@@ -1295,8 +1401,12 @@
         <v>1.0076357099921205</v>
       </c>
       <c r="F22" s="1"/>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G22">
+        <f t="shared" si="1"/>
+        <v>0.1957958455006272</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>21</v>
       </c>
@@ -1308,8 +1418,12 @@
         <v>0.95504589857130218</v>
       </c>
       <c r="F23" s="1"/>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G23">
+        <f t="shared" si="1"/>
+        <v>0.67834296674836536</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>22</v>
       </c>
@@ -1321,8 +1435,12 @@
         <v>1.0313251059388946</v>
       </c>
       <c r="F24" s="1"/>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G24">
+        <f t="shared" si="1"/>
+        <v>0.23420719212422481</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>23</v>
       </c>
@@ -1334,8 +1452,12 @@
         <v>0.99999999733047806</v>
       </c>
       <c r="F25" s="1"/>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G25">
+        <f t="shared" si="1"/>
+        <v>1.9999998942496928</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>24</v>
       </c>
@@ -1347,8 +1469,12 @@
         <v>1.0000000026695219</v>
       </c>
       <c r="F26" s="1"/>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G26">
+        <f t="shared" si="1"/>
+        <v>0.25000000998063915</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>25</v>
       </c>
@@ -1360,8 +1486,12 @@
         <v>0.58496249538211187</v>
       </c>
       <c r="F27" s="1"/>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G27">
+        <f t="shared" si="1"/>
+        <v>4.7829954926336554E-4</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>26</v>
       </c>
@@ -1373,8 +1503,12 @@
         <v>1.709511279572963</v>
       </c>
       <c r="F28" s="1"/>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G28">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>27</v>
       </c>
@@ -1384,7 +1518,7 @@
       <c r="D29" s="1"/>
       <c r="F29" s="1"/>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>2</v>
       </c>
@@ -1394,7 +1528,7 @@
       <c r="D30" s="1"/>
       <c r="F30" s="1"/>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>0</v>
       </c>
@@ -1404,7 +1538,7 @@
       <c r="D31" s="1"/>
       <c r="F31" s="1"/>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>1</v>
       </c>
@@ -1821,7 +1955,7 @@
         <v>1.1999969500000001</v>
       </c>
       <c r="D69" s="1">
-        <f t="shared" ref="D69:D132" si="1">LOG10(ABS((B70-B69)/(B69-B68)))/LOG10(ABS((B69-B68)/(B68-B67)))</f>
+        <f t="shared" ref="D69:D132" si="2">LOG10(ABS((B70-B69)/(B69-B68)))/LOG10(ABS((B69-B68)/(B68-B67)))</f>
         <v>1.000000000010496</v>
       </c>
     </row>
@@ -1833,7 +1967,7 @@
         <v>1.2000045800000001</v>
       </c>
       <c r="D70" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1.0018920593717329</v>
       </c>
     </row>
@@ -1845,7 +1979,7 @@
         <v>1.20000839</v>
       </c>
       <c r="D71" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.99433701481292647</v>
       </c>
     </row>
@@ -1893,7 +2027,7 @@
         <v>1.11150086</v>
       </c>
       <c r="D76" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.99441223252583077</v>
       </c>
     </row>
@@ -1905,7 +2039,7 @@
         <v>1.1410565699999999</v>
       </c>
       <c r="D77" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.99704771121773972</v>
       </c>
     </row>
@@ -1917,7 +2051,7 @@
         <v>1.16072727</v>
       </c>
       <c r="D78" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.99836197508579971</v>
       </c>
     </row>
@@ -1929,7 +2063,7 @@
         <v>1.1738277699999999</v>
       </c>
       <c r="D79" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.99905247447649193</v>
       </c>
     </row>
@@ -1941,7 +2075,7 @@
         <v>1.1825559400000001</v>
       </c>
       <c r="D80" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.99943595504369631</v>
       </c>
     </row>
@@ -1953,7 +2087,7 @@
         <v>1.1883723900000001</v>
       </c>
       <c r="D81" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.99964445138938185</v>
       </c>
     </row>
@@ -1965,7 +2099,7 @@
         <v>1.1922490299999999</v>
       </c>
       <c r="D82" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.99977546713238841</v>
       </c>
     </row>
@@ -1977,7 +2111,7 @@
         <v>1.1948330300000001</v>
       </c>
       <c r="D83" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.99987443133478793</v>
       </c>
     </row>
@@ -1989,7 +2123,7 @@
         <v>1.1965555000000001</v>
       </c>
       <c r="D84" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.99989743616544768</v>
       </c>
     </row>
@@ -2001,7 +2135,7 @@
         <v>1.19770373</v>
       </c>
       <c r="D85" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.99993916254639892</v>
       </c>
     </row>
@@ -2013,7 +2147,7 @@
         <v>1.19846918</v>
       </c>
       <c r="D86" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.99993020088261064</v>
       </c>
     </row>
@@ -2025,7 +2159,7 @@
         <v>1.19897947</v>
       </c>
       <c r="D87" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1.0000483314407185</v>
       </c>
     </row>
@@ -2037,7 +2171,7 @@
         <v>1.1993196500000001</v>
       </c>
       <c r="D88" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.99986709842494048</v>
       </c>
     </row>
@@ -2049,7 +2183,7 @@
         <v>1.19954644</v>
       </c>
       <c r="D89" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1.0000906277611745</v>
       </c>
     </row>
@@ -2061,7 +2195,7 @@
         <v>1.19969763</v>
       </c>
       <c r="D90" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1.0000271881506486</v>
       </c>
     </row>
@@ -2073,7 +2207,7 @@
         <v>1.19979842</v>
       </c>
       <c r="D91" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.99967377711751204</v>
       </c>
     </row>
@@ -2085,7 +2219,7 @@
         <v>1.19986562</v>
       </c>
       <c r="D92" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.99969415751818103</v>
       </c>
     </row>
@@ -2097,7 +2231,7 @@
         <v>1.1999104300000001</v>
       </c>
       <c r="D93" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1.0016523906667365</v>
       </c>
     </row>
@@ -2109,7 +2243,7 @@
         <v>1.19994029</v>
       </c>
       <c r="D94" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.99354320416817565</v>
       </c>
     </row>
@@ -2121,7 +2255,7 @@
         <v>1.19996024</v>
       </c>
       <c r="D95" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1.0053917921014268</v>
       </c>
     </row>
@@ -2133,7 +2267,7 @@
         <v>1.19997354</v>
       </c>
       <c r="D96" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.91434952894211785</v>
       </c>
     </row>
@@ -2145,7 +2279,7 @@
         <v>1.1999827199999999</v>
       </c>
       <c r="D97" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1.2015812995727355</v>
       </c>
     </row>
@@ -2157,7 +2291,7 @@
         <v>1.1999886</v>
       </c>
       <c r="D98" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.60543648757197799</v>
       </c>
     </row>
@@ -2169,7 +2303,7 @@
         <v>1.19999309</v>
       </c>
       <c r="D99" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.34596339279679</v>
       </c>
     </row>
@@ -2181,7 +2315,7 @@
         <v>1.19999718</v>
       </c>
       <c r="D100" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>-19.167695190723716</v>
       </c>
     </row>
@@ -2193,7 +2327,7 @@
         <v>1.2000216399999999</v>
       </c>
       <c r="D101" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>-0.69397970537710474</v>
       </c>
     </row>
@@ -2205,7 +2339,7 @@
         <v>1.20001457</v>
       </c>
       <c r="D102" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.75785206251505832</v>
       </c>
     </row>
@@ -2217,7 +2351,7 @@
         <v>1.2000118099999999</v>
       </c>
       <c r="D103" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>-1.1493274013873973E-2</v>
       </c>
     </row>
@@ -2301,7 +2435,7 @@
         <v>1.4526118100000001</v>
       </c>
       <c r="D112" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>-0.38810892147735987</v>
       </c>
     </row>
@@ -2313,7 +2447,7 @@
         <v>1.37561518</v>
       </c>
       <c r="D113" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>-0.56104969445066666</v>
       </c>
     </row>
@@ -2325,7 +2459,7 @@
         <v>1.33671826</v>
       </c>
       <c r="D114" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.16767567274128226</v>
       </c>
     </row>
@@ -2337,7 +2471,7 @@
         <v>1.3020294100000001</v>
       </c>
       <c r="D115" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2.9916506047183717</v>
       </c>
     </row>
@@ -2349,7 +2483,7 @@
         <v>1.27740141</v>
       </c>
       <c r="D116" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.74892479248202659</v>
       </c>
     </row>
@@ -2361,7 +2495,7 @@
         <v>1.25834599</v>
       </c>
       <c r="D117" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1.1300886173019626</v>
       </c>
     </row>
@@ -2373,7 +2507,7 @@
         <v>1.24408615</v>
       </c>
       <c r="D118" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.95614992765422424</v>
       </c>
     </row>
@@ -2385,7 +2519,7 @@
         <v>1.23327849</v>
       </c>
       <c r="D119" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1.0180548899614226</v>
       </c>
     </row>
@@ -2397,7 +2531,7 @@
         <v>1.2251281599999999</v>
       </c>
       <c r="D120" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.99354297701954686</v>
       </c>
     </row>
@@ -2409,7 +2543,7 @@
         <v>1.2189705799999999</v>
       </c>
       <c r="D121" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1.0028271061596268</v>
       </c>
     </row>
@@ -2421,7 +2555,7 @@
         <v>1.21432221</v>
       </c>
       <c r="D122" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.99919353034877323</v>
       </c>
     </row>
@@ -2433,7 +2567,7 @@
         <v>1.2108123500000001</v>
       </c>
       <c r="D123" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1.0005124488109374</v>
       </c>
     </row>
@@ -2445,7 +2579,7 @@
         <v>1.2081625300000001</v>
       </c>
       <c r="D124" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.99998267506233729</v>
       </c>
     </row>
@@ -2457,7 +2591,7 @@
         <v>1.206162</v>
       </c>
       <c r="D125" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1.0001570194349649</v>
       </c>
     </row>
@@ -2469,7 +2603,7 @@
         <v>1.2046517299999999</v>
       </c>
       <c r="D126" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1.0000174564705926</v>
       </c>
     </row>
@@ -2481,7 +2615,7 @@
         <v>1.20351158</v>
       </c>
       <c r="D127" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1.0001026987268529</v>
       </c>
     </row>
@@ -2493,7 +2627,7 @@
         <v>1.20265087</v>
       </c>
       <c r="D128" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.99998963021750553</v>
       </c>
     </row>
@@ -2505,7 +2639,7 @@
         <v>1.2020011100000001</v>
       </c>
       <c r="D129" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1.0001550976056053</v>
       </c>
     </row>
@@ -2517,7 +2651,7 @@
         <v>1.2015106200000001</v>
       </c>
       <c r="D130" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.99981238405270811</v>
       </c>
     </row>
@@ -2529,7 +2663,7 @@
         <v>1.20114034</v>
       </c>
       <c r="D131" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1.0001430383435215</v>
       </c>
     </row>
@@ -2541,7 +2675,7 @@
         <v>1.2008608199999999</v>
       </c>
       <c r="D132" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1.0001069866091734</v>
       </c>
     </row>
@@ -2553,7 +2687,7 @@
         <v>1.20064982</v>
       </c>
       <c r="D133" s="1">
-        <f t="shared" ref="D133:D175" si="2">LOG10(ABS((B134-B133)/(B133-B132)))/LOG10(ABS((B133-B132)/(B132-B131)))</f>
+        <f t="shared" ref="D133:D174" si="3">LOG10(ABS((B134-B133)/(B133-B132)))/LOG10(ABS((B133-B132)/(B132-B131)))</f>
         <v>0.99992447367460091</v>
       </c>
     </row>
@@ -2565,7 +2699,7 @@
         <v>1.2004905400000001</v>
       </c>
       <c r="D134" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.99992688543327846</v>
       </c>
     </row>
@@ -2577,7 +2711,7 @@
         <v>1.2003702999999999</v>
       </c>
       <c r="D135" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.99995375317921353</v>
       </c>
     </row>
@@ -2589,7 +2723,7 @@
         <v>1.20027953</v>
       </c>
       <c r="D136" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1.0001502704406171</v>
       </c>
     </row>
@@ -2601,7 +2735,7 @@
         <v>1.2002110100000001</v>
       </c>
       <c r="D137" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1.000277231827341</v>
       </c>
     </row>
@@ -2613,7 +2747,7 @@
         <v>1.20015929</v>
       </c>
       <c r="D138" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.99900653861522737</v>
       </c>
     </row>
@@ -2625,7 +2759,7 @@
         <v>1.2001202399999999</v>
       </c>
       <c r="D139" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1.0040828531013901</v>
       </c>
     </row>
@@ -2637,7 +2771,7 @@
         <v>1.20009079</v>
       </c>
       <c r="D140" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.9920382414738883</v>
       </c>
     </row>
@@ -2649,7 +2783,7 @@
         <v>1.20006853</v>
       </c>
       <c r="D141" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1.0117798340506909</v>
       </c>
     </row>
@@ -2661,7 +2795,7 @@
         <v>1.20005176</v>
       </c>
       <c r="D142" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1.0095162219431557</v>
       </c>
     </row>
@@ -2673,7 +2807,7 @@
         <v>1.20003916</v>
       </c>
       <c r="D143" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.95481261456142774</v>
       </c>
     </row>
@@ -2685,7 +2819,7 @@
         <v>1.2000295700000001</v>
       </c>
       <c r="D144" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1.1584916601317961</v>
       </c>
     </row>
@@ -2697,7 +2831,7 @@
         <v>1.2000225799999999</v>
       </c>
       <c r="D145" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.73515624528251922</v>
       </c>
     </row>
@@ -2709,7 +2843,7 @@
         <v>1.2000170400000001</v>
       </c>
       <c r="D146" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1.3794917607793387</v>
       </c>
     </row>
@@ -2721,7 +2855,7 @@
         <v>1.2000130200000001</v>
       </c>
       <c r="D147" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>-7.7467283242593776E-3</v>
       </c>
     </row>
@@ -2733,7 +2867,7 @@
         <v>1.2000089899999999</v>
       </c>
       <c r="D148" s="1" t="e">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>#NUM!</v>
       </c>
     </row>
@@ -2784,7 +2918,7 @@
         <v>13</v>
       </c>
       <c r="D154" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>-0.13025600124513445</v>
       </c>
     </row>
@@ -2796,7 +2930,7 @@
         <v>1.3</v>
       </c>
       <c r="D155" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>10.385261528026406</v>
       </c>
     </row>
@@ -2808,7 +2942,7 @@
         <v>1.5941176500000001</v>
       </c>
       <c r="D156" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.71724949110468728</v>
       </c>
     </row>
@@ -2820,7 +2954,7 @@
         <v>1.49282165</v>
       </c>
       <c r="D157" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>2.4828626856435667</v>
       </c>
     </row>
@@ -2832,7 +2966,7 @@
         <v>1.50000296</v>
       </c>
       <c r="D158" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>2.9449673504215363</v>
       </c>
     </row>
@@ -2886,7 +3020,7 @@
         <v>1.4864316</v>
       </c>
       <c r="D164" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>8.6055675226816941</v>
       </c>
     </row>
@@ -2898,7 +3032,7 @@
         <v>1.4999600900000001</v>
       </c>
       <c r="D165" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>3.2030539824917916</v>
       </c>
     </row>
@@ -2946,7 +3080,7 @@
         <v>1.876493</v>
       </c>
       <c r="D170" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>-1.920569840998037</v>
       </c>
     </row>
@@ -2958,7 +3092,7 @@
         <v>1.5492468399999999</v>
       </c>
       <c r="D171" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>3.1380468802751063</v>
       </c>
     </row>
@@ -2970,7 +3104,7 @@
         <v>1.4523931400000001</v>
       </c>
       <c r="D172" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.58307618412838214</v>
       </c>
     </row>
@@ -2982,7 +3116,7 @@
         <v>1.50001538</v>
       </c>
       <c r="D173" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>11.309911626267883</v>
       </c>
     </row>
@@ -2994,7 +3128,7 @@
         <v>1.49999986</v>
       </c>
       <c r="D174" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.58641001051378594</v>
       </c>
     </row>

</xml_diff>